<commit_message>
cette fois cest les bon fichier
</commit_message>
<xml_diff>
--- a/Modèle-audit-SEO.xlsx
+++ b/Modèle-audit-SEO.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="106">
   <si>
     <t xml:space="preserve">Catégorie</t>
   </si>
@@ -49,10 +49,10 @@
     <t xml:space="preserve">lang</t>
   </si>
   <si>
-    <t xml:space="preserve">la lang est en default </t>
-  </si>
-  <si>
-    <t xml:space="preserve">mettre une langue definie </t>
+    <t xml:space="preserve">la lang est en défault </t>
+  </si>
+  <si>
+    <t xml:space="preserve">mettre une langue définie </t>
   </si>
   <si>
     <t xml:space="preserve">mettre FR </t>
@@ -61,7 +61,7 @@
     <t xml:space="preserve">le titre de la page</t>
   </si>
   <si>
-    <t xml:space="preserve">le titre de la page cest un point </t>
+    <t xml:space="preserve">le titre de la page c’est un point </t>
   </si>
   <si>
     <t xml:space="preserve">mettre un titre qui correspond a la page </t>
@@ -70,19 +70,19 @@
     <t xml:space="preserve">mettre la chouette agence </t>
   </si>
   <si>
-    <t xml:space="preserve">mot repetitif dans la balise keyword</t>
+    <t xml:space="preserve">mot répétitif dans la balise keyword</t>
   </si>
   <si>
     <t xml:space="preserve">la balise keyword est mal utiliser </t>
   </si>
   <si>
-    <t xml:space="preserve">mettre quelque keyword sans reptition</t>
+    <t xml:space="preserve">mettre quelque keyword sans répétition</t>
   </si>
   <si>
     <t xml:space="preserve">div keyword </t>
   </si>
   <si>
-    <t xml:space="preserve">il ya une div keyword qui permet de mettre en invisible des mots cle </t>
+    <t xml:space="preserve">il y a une div keyword qui permet de mettre en invisible des mots clé</t>
   </si>
   <si>
     <t xml:space="preserve">ne rien mettre en invisible </t>
@@ -100,7 +100,7 @@
     <t xml:space="preserve">il y  a des mots clé dans le alt</t>
   </si>
   <si>
-    <t xml:space="preserve">pas mettre de mots cle dans les alt </t>
+    <t xml:space="preserve">pas mettre de mots clé dans les alt </t>
   </si>
   <si>
     <t xml:space="preserve">mettre logo de la chouette agence </t>
@@ -112,7 +112,7 @@
     <t xml:space="preserve">le titre de la page 2</t>
   </si>
   <si>
-    <t xml:space="preserve">le titre de la page 2 cest la page 2</t>
+    <t xml:space="preserve">le titre de la page 2 c’est la page 2</t>
   </si>
   <si>
     <t xml:space="preserve">mettre contact</t>
@@ -121,7 +121,7 @@
     <t xml:space="preserve">accessibilité</t>
   </si>
   <si>
-    <t xml:space="preserve">police de la balise p </t>
+    <t xml:space="preserve">police de la balise &lt;p&gt; </t>
   </si>
   <si>
     <t xml:space="preserve">la police est trop petite </t>
@@ -139,37 +139,205 @@
     <t xml:space="preserve">les image sont trop grande </t>
   </si>
   <si>
-    <t xml:space="preserve">rogner les image ou reussir a les adapter correctement </t>
-  </si>
-  <si>
-    <t xml:space="preserve">reduire la tailles des image </t>
+    <t xml:space="preserve">rogner les image ou réussir a les adapter correctement </t>
+  </si>
+  <si>
+    <t xml:space="preserve">réduire la tailles des image </t>
   </si>
   <si>
     <t xml:space="preserve">image texte</t>
   </si>
   <si>
-    <t xml:space="preserve">cest une image qui pourrais simplement etre un paragraphe </t>
-  </si>
-  <si>
-    <t xml:space="preserve">de pas mettre dimage texte </t>
-  </si>
-  <si>
-    <t xml:space="preserve">reecrire limage </t>
+    <t xml:space="preserve">c’est une image qui pourrais simplement être un paragraphe </t>
+  </si>
+  <si>
+    <t xml:space="preserve">de pas mettre d’image texte </t>
+  </si>
+  <si>
+    <t xml:space="preserve">réécrire limage </t>
   </si>
   <si>
     <t xml:space="preserve">accessibilité et seo</t>
   </si>
   <si>
-    <t xml:space="preserve">le href des reseau sociaux </t>
-  </si>
-  <si>
-    <t xml:space="preserve">le href est le lien de lacceuil de la page </t>
-  </si>
-  <si>
-    <t xml:space="preserve">ne pas mettre nimporte quel lien </t>
-  </si>
-  <si>
-    <t xml:space="preserve">mettre un # si il ny a pas de lien emmenant a la bonne page en attendant </t>
+    <t xml:space="preserve">le href des réseau sociaux </t>
+  </si>
+  <si>
+    <t xml:space="preserve">le href est le lien de l’accueil de la page </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ne pas mettre n’importe quel lien </t>
+  </si>
+  <si>
+    <t xml:space="preserve">mettre un # si il n’y a pas de lien emmenant a la bonne page en attendant </t>
+  </si>
+  <si>
+    <t xml:space="preserve">balise description</t>
+  </si>
+  <si>
+    <t xml:space="preserve">balise description vide</t>
+  </si>
+  <si>
+    <t xml:space="preserve">remplir la balise avec un mots clé, rappeler le nom de marque présenter des avantage mettre des mots du champ lexical du sujet pour que google comprenne mieux le contexte</t>
+  </si>
+  <si>
+    <t xml:space="preserve">remplir la balise description </t>
+  </si>
+  <si>
+    <t xml:space="preserve">il n’y a pas google analytic </t>
+  </si>
+  <si>
+    <t xml:space="preserve">on ne peux pas suivre nos visiteur </t>
+  </si>
+  <si>
+    <t xml:space="preserve">suivre nos visiteur pour voir si notre trafic évolue </t>
+  </si>
+  <si>
+    <t xml:space="preserve">installer google analytic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">balise &lt;li&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">il y a un balise &lt;li&gt; inutile </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ne pas mettre de balise inutile </t>
+  </si>
+  <si>
+    <t xml:space="preserve">supprimer cette balise</t>
+  </si>
+  <si>
+    <t xml:space="preserve">responsive</t>
+  </si>
+  <si>
+    <t xml:space="preserve">site non responsive des éléments sont caché et le site n’est pas beau à regarder </t>
+  </si>
+  <si>
+    <t xml:space="preserve">adapter les site en responsive </t>
+  </si>
+  <si>
+    <t xml:space="preserve">adapter le site </t>
+  </si>
+  <si>
+    <t xml:space="preserve">h2 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">mauvaise sémantique le premier h2 n’est pas vraiment un titre </t>
+  </si>
+  <si>
+    <t xml:space="preserve">respecter la sémantique </t>
+  </si>
+  <si>
+    <t xml:space="preserve">mettre une balise &lt;p&gt; a la place de &lt;h2&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mauvaise traduction de l’espace et apostrophe en html </t>
+  </si>
+  <si>
+    <t xml:space="preserve">dans le code html il y a des endroit ou il y a écrit « &amp;rsquo; » ou « &amp;nbsp; »</t>
+  </si>
+  <si>
+    <t xml:space="preserve">faire attention a la traduction en html </t>
+  </si>
+  <si>
+    <t xml:space="preserve">remplacer par un espace ou une apostrophe </t>
+  </si>
+  <si>
+    <t xml:space="preserve">balise &lt;br&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">il y a des balises &lt;br&gt; qui ne servent a rien </t>
+  </si>
+  <si>
+    <t xml:space="preserve">couleur des h2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">la couleur des h2 n’est pas assez lisible car c’est du orange sur du orange </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Faire en sorte que se soit lisible </t>
+  </si>
+  <si>
+    <t xml:space="preserve">changer la couleur en noir </t>
+  </si>
+  <si>
+    <t xml:space="preserve">les alt des images </t>
+  </si>
+  <si>
+    <t xml:space="preserve">les alt des images ne décrivent pas assez bien les images </t>
+  </si>
+  <si>
+    <t xml:space="preserve">les alt des images sont des description d’images il faut donc les décrire </t>
+  </si>
+  <si>
+    <t xml:space="preserve">changer les alt </t>
+  </si>
+  <si>
+    <t xml:space="preserve">lien vers page 2 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">il y a beaucoup de lien emmenant sur la page 2 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">faire attention à ne pas mettre trop de lien vers le même endroit </t>
+  </si>
+  <si>
+    <t xml:space="preserve">peut être en supprimer 1 lien</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;li&gt; du header page 2 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">les &lt;li&gt; du header ne sont pas accessible </t>
+  </si>
+  <si>
+    <t xml:space="preserve">vérifier l’accessibilité de tous les boutons</t>
+  </si>
+  <si>
+    <t xml:space="preserve">adapter le toogle navigation en responsive et le supprimer en desktop </t>
+  </si>
+  <si>
+    <t xml:space="preserve">h1 et p</t>
+  </si>
+  <si>
+    <t xml:space="preserve">le &lt;h1&gt; et &lt;p&gt; sont invisible </t>
+  </si>
+  <si>
+    <t xml:space="preserve">vérifier que les texte soient bien affiché</t>
+  </si>
+  <si>
+    <t xml:space="preserve">faire en sorte que le &lt;h1&gt; et &lt;p&gt; soient affiché </t>
+  </si>
+  <si>
+    <t xml:space="preserve">comment nous avez-vous connu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dans le input le type est email </t>
+  </si>
+  <si>
+    <t xml:space="preserve">vérifier que les input soient cohérent </t>
+  </si>
+  <si>
+    <t xml:space="preserve">remplacer le type email par type texte </t>
+  </si>
+  <si>
+    <t xml:space="preserve">bouton invisible </t>
+  </si>
+  <si>
+    <t xml:space="preserve">il y a un bouton invisible qui permet de remonter en haut de la page il est inutile </t>
+  </si>
+  <si>
+    <t xml:space="preserve">supprimer le bouton</t>
+  </si>
+  <si>
+    <t xml:space="preserve">réseau sociaux invisible</t>
+  </si>
+  <si>
+    <t xml:space="preserve">les boutons des réseau sociaux son inutilisable car invisible </t>
+  </si>
+  <si>
+    <t xml:space="preserve">les mettre visible </t>
   </si>
 </sst>
 </file>
@@ -232,7 +400,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -245,12 +413,32 @@
         <bgColor rgb="FF993366"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFB4C7DC"/>
+        <bgColor rgb="FFCCCCFF"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="hair"/>
+      <right style="hair"/>
+      <top style="hair"/>
+      <bottom style="hair"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right/>
+      <top style="thin"/>
       <bottom/>
       <diagonal/>
     </border>
@@ -280,7 +468,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="12">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -299,6 +487,34 @@
     </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -326,7 +542,7 @@
       <rgbColor rgb="FF808000"/>
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FFB4C7DC"/>
       <rgbColor rgb="FF808080"/>
       <rgbColor rgb="FF9999FF"/>
       <rgbColor rgb="FF7030A0"/>
@@ -381,16 +597,16 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B22" activeCellId="0" sqref="B22"/>
+      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.30078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.32421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="33.84"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="57.59"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="62.69"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="61.07"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="29.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="50.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="55.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="35.23"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="25.49"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="7" style="0" width="10.57"/>
   </cols>
@@ -441,207 +657,550 @@
       </c>
       <c r="E2" s="4"/>
     </row>
-    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+    <row r="3" customFormat="false" ht="32.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="C3" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="D3" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="7" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="F3" s="6"/>
+    </row>
+    <row r="4" customFormat="false" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="C4" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="0" t="s">
+      <c r="D4" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="7" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="F4" s="6"/>
+    </row>
+    <row r="5" customFormat="false" ht="34.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="C5" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="0" t="s">
+      <c r="D5" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="E5" s="4"/>
-    </row>
-    <row r="6" customFormat="false" ht="18.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="E5" s="7"/>
+      <c r="F5" s="6"/>
+    </row>
+    <row r="6" customFormat="false" ht="49.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="0" t="s">
+      <c r="C6" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="D6" s="0" t="s">
+      <c r="D6" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="E6" s="7" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+      <c r="F6" s="6"/>
+    </row>
+    <row r="7" customFormat="false" ht="48.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="B7" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="0" t="s">
+      <c r="C7" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="D7" s="0" t="s">
+      <c r="D7" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="E7" s="7" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+      <c r="F7" s="6"/>
+    </row>
+    <row r="8" customFormat="false" ht="47" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B8" s="0" t="s">
+      <c r="B8" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="0" t="s">
+      <c r="C8" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="D8" s="0" t="s">
+      <c r="D8" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="E8" s="4" t="s">
+      <c r="E8" s="7" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+      <c r="F8" s="6"/>
+    </row>
+    <row r="9" customFormat="false" ht="47" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="B9" s="0" t="s">
+      <c r="B9" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="C9" s="0" t="s">
+      <c r="C9" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="D9" s="0" t="s">
+      <c r="D9" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="E9" s="4" t="s">
+      <c r="E9" s="7" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+      <c r="F9" s="6"/>
+    </row>
+    <row r="10" customFormat="false" ht="44" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="B10" s="0" t="s">
+      <c r="B10" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="C10" s="0" t="s">
+      <c r="C10" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="D10" s="0" t="s">
+      <c r="D10" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="E10" s="4" t="s">
+      <c r="E10" s="7" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
+      <c r="F10" s="6"/>
+    </row>
+    <row r="11" customFormat="false" ht="47" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="B11" s="0" t="s">
+      <c r="B11" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="C11" s="0" t="s">
+      <c r="C11" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="D11" s="0" t="s">
+      <c r="D11" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="E11" s="4" t="s">
+      <c r="E11" s="7" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
+      <c r="F11" s="6"/>
+    </row>
+    <row r="12" customFormat="false" ht="51.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="B12" s="0" t="s">
+      <c r="B12" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="C12" s="0" t="s">
+      <c r="C12" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="D12" s="0" t="s">
+      <c r="D12" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="E12" s="0" t="s">
+      <c r="E12" s="6" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="E13" s="4"/>
-    </row>
-    <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="E14" s="4"/>
-    </row>
-    <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="E15" s="4"/>
-    </row>
-    <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+      <c r="F12" s="6"/>
+    </row>
+    <row r="13" customFormat="false" ht="49.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A13" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="E13" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="F13" s="8"/>
+    </row>
+    <row r="14" customFormat="false" ht="41" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A14" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="F14" s="6"/>
+    </row>
+    <row r="15" customFormat="false" ht="43.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A15" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="F15" s="6"/>
+    </row>
+    <row r="16" customFormat="false" ht="47.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A16" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="F16" s="6"/>
+    </row>
+    <row r="17" customFormat="false" ht="46.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A17" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="F17" s="6"/>
+    </row>
+    <row r="18" customFormat="false" ht="38.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A18" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="F18" s="6"/>
+    </row>
+    <row r="19" customFormat="false" ht="38.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A19" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="F19" s="6"/>
+    </row>
+    <row r="20" customFormat="false" ht="32.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A20" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="F20" s="6"/>
+    </row>
+    <row r="21" customFormat="false" ht="32.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A21" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="F21" s="6"/>
+    </row>
+    <row r="22" customFormat="false" ht="41.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A22" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="E22" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="F22" s="6"/>
+    </row>
+    <row r="23" customFormat="false" ht="33.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A23" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="D23" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="F23" s="6"/>
+    </row>
+    <row r="24" customFormat="false" ht="32.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A24" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="F24" s="6"/>
+    </row>
+    <row r="25" customFormat="false" ht="38.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A25" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="D25" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="E25" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="F25" s="6"/>
+    </row>
+    <row r="26" customFormat="false" ht="45.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A26" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="D26" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="E26" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="F26" s="6"/>
+    </row>
+    <row r="27" customFormat="false" ht="48.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A27" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="D27" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="E27" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="F27" s="6"/>
+    </row>
+    <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A28" s="11"/>
+      <c r="B28" s="11"/>
+      <c r="C28" s="11"/>
+      <c r="D28" s="11"/>
+      <c r="E28" s="11"/>
+      <c r="F28" s="11"/>
+    </row>
+    <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A29" s="11"/>
+      <c r="B29" s="11"/>
+      <c r="C29" s="11"/>
+      <c r="D29" s="11"/>
+      <c r="E29" s="11"/>
+      <c r="F29" s="11"/>
+    </row>
+    <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A30" s="11"/>
+      <c r="B30" s="11"/>
+      <c r="C30" s="11"/>
+      <c r="D30" s="11"/>
+      <c r="E30" s="11"/>
+      <c r="F30" s="11"/>
+    </row>
+    <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A31" s="11"/>
+      <c r="B31" s="11"/>
+      <c r="C31" s="11"/>
+      <c r="D31" s="11"/>
+      <c r="E31" s="11"/>
+      <c r="F31" s="11"/>
+    </row>
+    <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A32" s="11"/>
+      <c r="B32" s="11"/>
+      <c r="C32" s="11"/>
+      <c r="D32" s="11"/>
+      <c r="E32" s="11"/>
+      <c r="F32" s="11"/>
+    </row>
+    <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A33" s="11"/>
+      <c r="B33" s="11"/>
+      <c r="C33" s="11"/>
+      <c r="D33" s="11"/>
+      <c r="E33" s="11"/>
+      <c r="F33" s="11"/>
+    </row>
+    <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A34" s="11"/>
+      <c r="B34" s="11"/>
+      <c r="C34" s="11"/>
+      <c r="D34" s="11"/>
+      <c r="E34" s="11"/>
+      <c r="F34" s="11"/>
+    </row>
+    <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A35" s="11"/>
+      <c r="B35" s="11"/>
+      <c r="C35" s="11"/>
+      <c r="D35" s="11"/>
+      <c r="E35" s="11"/>
+      <c r="F35" s="11"/>
+    </row>
+    <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A36" s="11"/>
+      <c r="B36" s="11"/>
+      <c r="C36" s="11"/>
+      <c r="D36" s="11"/>
+      <c r="E36" s="11"/>
+      <c r="F36" s="11"/>
+    </row>
+    <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A37" s="11"/>
+      <c r="B37" s="11"/>
+      <c r="C37" s="11"/>
+      <c r="D37" s="11"/>
+      <c r="E37" s="11"/>
+      <c r="F37" s="11"/>
+    </row>
+    <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A38" s="11"/>
+      <c r="B38" s="11"/>
+      <c r="C38" s="11"/>
+      <c r="D38" s="11"/>
+      <c r="E38" s="11"/>
+      <c r="F38" s="11"/>
+    </row>
+    <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A39" s="11"/>
+      <c r="B39" s="11"/>
+      <c r="C39" s="11"/>
+      <c r="D39" s="11"/>
+      <c r="E39" s="11"/>
+      <c r="F39" s="11"/>
+    </row>
     <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>